<commit_message>
Cambios Material y Reporte de Equipment Daily rent
</commit_message>
<xml_diff>
--- a/AVT_TRAKING-b5a19f52c2a889d8592336db032ecf143043f8f5/AVT_TRAKING/AVT_TRAKING/Documents/InvoicePieces.xlsx
+++ b/AVT_TRAKING-b5a19f52c2a889d8592336db032ecf143043f8f5/AVT_TRAKING/AVT_TRAKING/Documents/InvoicePieces.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Desktop\Respaldo\Images\Datos Andres\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713F6DAB-6777-44FA-B486-A7114DAAC912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12579EE-93E7-45BF-B2BF-BA4B59092DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{38B5D577-474C-4399-9CA6-7E2D0DD88AA4}"/>
+    <workbookView xWindow="7815" yWindow="1125" windowWidth="12555" windowHeight="5895" activeTab="1" xr2:uid="{38B5D577-474C-4399-9CA6-7E2D0DD88AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Pieces" sheetId="3" r:id="rId1"/>
+    <sheet name="SRLs" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="Consulta_desde_VRT_TRAKING" localSheetId="0" hidden="1">Pieces!$A$5:$L$14</definedName>
+    <definedName name="Consulta_desde_VRT_TRAKING" localSheetId="1" hidden="1">SRLs!$A$5:$H$7</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,14 +45,17 @@
   <connection id="2" xr16:uid="{358B69CF-9515-41AB-97DE-7160754EFFB3}" name="Consulta desde VRT_TRAKING" type="1" refreshedVersion="7" background="1" refreshOnLoad="1" saveData="1">
     <dbPr connection="DRIVER=SQL Server;SERVER=127.0.0.1;UID=isaac;Trusted_Connection=Yes;APP=Microsoft Office;WSID=DESKTOP-S806JIQ;DATABASE=VRT_TRAKING" command="SELECT InvoiceExcel.&quot;Labor WO / NERWORK #&quot;, InvoiceExcel.&quot;Type (O,M,T,C)&quot;, InvoiceExcel.&quot;Tag #&quot;, InvoiceExcel.Pieces, InvoiceExcel.UNIT, InvoiceExcel.Location, InvoiceExcel.&quot;Date UP&quot;, InvoiceExcel.&quot;Date Down&quot;, InvoiceExcel.&quot;Invoice Amount&quot;, InvoiceExcel.ACTIVEDAYS, InvoiceExcel.RDays, InvoiceExcel.Work_x000d__x000a_FROM VRT_TRAKING.dbo.InvoiceExcel InvoiceExcel_x000d__x000a_ORDER BY InvoiceExcel.&quot;Tag #&quot;"/>
   </connection>
-  <connection id="3" xr16:uid="{32D1275F-F463-4C03-B5B4-F70030FC115D}" odcFile="C:\Users\isaac\Documents\Mis archivos de origen de datos\localhost VRT_TRAKING product.odc" keepAlive="1" name="localhost VRT_TRAKING product" type="5" refreshedVersion="0" new="1" background="1">
+  <connection id="3" xr16:uid="{EE09C335-DAC7-4B93-B309-92AFA520840C}" name="Consulta desde VRT_TRAKING1" type="1" refreshedVersion="7" background="1" refreshOnLoad="1" saveData="1">
+    <dbPr connection="DRIVER=SQL Server;SERVER=127.0.0.1;UID=isaac;Trusted_Connection=Yes;APP=Microsoft Office;WSID=DESKTOP-S806JIQ;DATABASE=VRT_TRAKING" command="SELECT InvoiceExcelYOYOS.&quot;Labor WO / Network #&quot;, InvoiceExcelYOYOS.&quot;Type (O,M,T,C)&quot;, InvoiceExcelYOYOS.&quot;Tag #&quot;, InvoiceExcelYOYOS.Pieces, InvoiceExcelYOYOS.UNIT, InvoiceExcelYOYOS.Location, InvoiceExcelYOYOS.&quot;Date UP&quot;, InvoiceExcelYOYOS.&quot;Date Down&quot;_x000d__x000a_FROM VRT_TRAKING.dbo.InvoiceExcelYOYOS InvoiceExcelYOYOS_x000d__x000a_ORDER BY InvoiceExcelYOYOS.&quot;Tag #&quot;"/>
+  </connection>
+  <connection id="4" xr16:uid="{32D1275F-F463-4C03-B5B4-F70030FC115D}" odcFile="C:\Users\isaac\Documents\Mis archivos de origen de datos\localhost VRT_TRAKING product.odc" keepAlive="1" name="localhost VRT_TRAKING product" type="5" refreshedVersion="0" new="1" background="1">
     <dbPr connection="Provider=SQLOLEDB.1;Integrated Security=SSPI;Persist Security Info=True;Data Source=localhost;Use Procedure for Prepare=1;Auto Translate=True;Packet Size=4096;Workstation ID=DESKTOP-S806JIQ;Use Encryption for Data=False;Tag with column collation when possible=False;Initial Catalog=VRT_TRAKING" command="&quot;VRT_TRAKING&quot;.&quot;dbo&quot;.&quot;product&quot;" commandType="3"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
   <si>
     <t>Type (O,M,T,C)</t>
   </si>
@@ -167,6 +172,12 @@
   </si>
   <si>
     <t>CALCULATED COLUMNS FOR INEOS REVIEW</t>
+  </si>
+  <si>
+    <t>Labor WO / Network #</t>
+  </si>
+  <si>
+    <t>01/03/2022</t>
   </si>
 </sst>
 </file>
@@ -247,7 +258,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -255,37 +266,191 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -343,10 +508,27 @@
 </queryTable>
 </file>
 
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Consulta desde VRT_TRAKING" refreshOnLoad="1" connectionId="3" xr16:uid="{1802F3C1-AADA-4D73-96CF-EFC362334CA6}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
+  <queryTableRefresh nextId="9">
+    <queryTableFields count="8">
+      <queryTableField id="1" name="Labor WO / Network #" tableColumnId="1"/>
+      <queryTableField id="2" name="Type (O,M,T,C)" tableColumnId="2"/>
+      <queryTableField id="3" name="Tag #" tableColumnId="3"/>
+      <queryTableField id="4" name="Pieces" tableColumnId="4"/>
+      <queryTableField id="5" name="UNIT" tableColumnId="5"/>
+      <queryTableField id="6" name="Location" tableColumnId="6"/>
+      <queryTableField id="7" name="Date UP" tableColumnId="7"/>
+      <queryTableField id="8" name="Date Down" tableColumnId="8"/>
+    </queryTableFields>
+  </queryTableRefresh>
+</queryTable>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0D176718-B392-4A9D-9070-4B0EE3EA7DDC}" name="Tabla_Consulta_desde_VRT_TRAKING" displayName="Tabla_Consulta_desde_VRT_TRAKING" ref="A5:L15" tableType="queryTable" totalsRowCount="1" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0D176718-B392-4A9D-9070-4B0EE3EA7DDC}" name="Tabla_Consulta_desde_VRT_TRAKING" displayName="Tabla_Consulta_desde_VRT_TRAKING" ref="A5:L15" tableType="queryTable" totalsRowCount="1" headerRowDxfId="3">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A1400F7A-234C-4C8B-B435-3F88501FD8B7}" uniqueName="1" name="Labor WO / NERWORK #" queryTableFieldId="1" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{A1400F7A-234C-4C8B-B435-3F88501FD8B7}" uniqueName="1" name="Labor WO / NERWORK #" queryTableFieldId="1" dataDxfId="2" totalsRowDxfId="1"/>
     <tableColumn id="2" xr3:uid="{45B8D241-B5C8-4158-8A96-974711A7D544}" uniqueName="2" name="Type (O,M,T,C)" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{C55F0CFC-4D16-42B3-9FF5-44F287BD50D2}" uniqueName="3" name="Tag #" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{53007AC2-912B-487D-BC00-D1306BC03F21}" uniqueName="4" name="Pieces" queryTableFieldId="4"/>
@@ -358,6 +540,22 @@
     <tableColumn id="10" xr3:uid="{DE68B60D-1AE4-4C11-A2A6-E732056235A1}" uniqueName="10" name="ACTIVEDAYS" queryTableFieldId="10"/>
     <tableColumn id="11" xr3:uid="{0317DF1D-BAA4-408F-9374-DC661A60C2A9}" uniqueName="11" name="RDays" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{B3D51080-ABCC-4A29-9907-A25ECC1D4EA8}" uniqueName="12" name="Work" queryTableFieldId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{73862926-8285-4075-A361-43ED838ED5E3}" name="Tabla_Consulta_desde_VRT_TRAKING2" displayName="Tabla_Consulta_desde_VRT_TRAKING2" ref="A5:H7" tableType="queryTable" totalsRowShown="0" headerRowDxfId="0">
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{2EA742A4-85B8-41E8-A43C-9B606511EF3A}" uniqueName="1" name="Labor WO / Network #" queryTableFieldId="1"/>
+    <tableColumn id="2" xr3:uid="{ECA3E2F2-912D-47F5-A68D-7AECFB0A8DDC}" uniqueName="2" name="Type (O,M,T,C)" queryTableFieldId="2"/>
+    <tableColumn id="3" xr3:uid="{1D1F2BBA-F570-4E0C-A3F6-710B841B41F4}" uniqueName="3" name="Tag #" queryTableFieldId="3"/>
+    <tableColumn id="4" xr3:uid="{C3564F34-8235-4FF2-A010-859B81F89141}" uniqueName="4" name="Pieces" queryTableFieldId="4"/>
+    <tableColumn id="5" xr3:uid="{686B7D68-5E7C-4A8D-8B68-D18F3EA9C159}" uniqueName="5" name="UNIT" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{89F29ABA-EE6B-4AF0-8419-1A7EBACCBF46}" uniqueName="6" name="Location" queryTableFieldId="6"/>
+    <tableColumn id="7" xr3:uid="{9FABF2C0-9ACE-4852-9D05-2C062CFFB2BC}" uniqueName="7" name="Date UP" queryTableFieldId="7"/>
+    <tableColumn id="8" xr3:uid="{ABE7E7C8-08F7-4567-A147-D9B7B542BA5E}" uniqueName="8" name="Date Down" queryTableFieldId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -660,15 +858,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DBB563-4785-449F-AAF5-1BCA63F1C3B4}">
-  <dimension ref="A1:M35"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
@@ -680,63 +878,76 @@
     <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="I1" s="4" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="J1" s="5">
-        <v>44652</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="I2" s="4" t="s">
+      <c r="J1" s="21">
+        <v>44593</v>
+      </c>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="5">
-        <v>44661</v>
-      </c>
-      <c r="K2" s="6">
+      <c r="J2" s="24">
+        <v>44620</v>
+      </c>
+      <c r="K2" s="25">
         <f>J2-(J1-1)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="18"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="10"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="K4" t="s">
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="28" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="29"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
@@ -774,8 +985,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
@@ -812,8 +1023,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
@@ -850,8 +1061,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -888,8 +1099,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -926,11 +1137,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C10" t="s">
@@ -964,8 +1175,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B11" t="s">
@@ -1002,8 +1213,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B12" t="s">
@@ -1040,8 +1251,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
@@ -1078,8 +1289,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
@@ -1116,78 +1327,247 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="6"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="6"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
+      <c r="A18" s="6"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
+      <c r="A19" s="6"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
+      <c r="A20" s="6"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
+      <c r="A21" s="6"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
+      <c r="A22" s="6"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9"/>
+      <c r="A23" s="6"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9"/>
+      <c r="A24" s="6"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="6"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="9"/>
+      <c r="A26" s="6"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
+      <c r="A27" s="6"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
+      <c r="A28" s="6"/>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+      <c r="A29" s="6"/>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="9"/>
+      <c r="A30" s="6"/>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="9"/>
+      <c r="A31" s="6"/>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="9"/>
+      <c r="A32" s="6"/>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="9"/>
+      <c r="A33" s="6"/>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="9"/>
+      <c r="A34" s="6"/>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9"/>
+      <c r="A35" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="K4:O4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F57257B-8A29-41E9-A359-4D17BE936CD4}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J1" s="13">
+        <v>44593</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="J2" s="16">
+        <v>44620</v>
+      </c>
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="18"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="20"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A4:F4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
(Ejecutar desde la 4830) Reporte de Equipment,excel Invoice,Reporte Material
</commit_message>
<xml_diff>
--- a/AVT_TRAKING-b5a19f52c2a889d8592336db032ecf143043f8f5/AVT_TRAKING/AVT_TRAKING/Documents/InvoicePieces.xlsx
+++ b/AVT_TRAKING-b5a19f52c2a889d8592336db032ecf143043f8f5/AVT_TRAKING/AVT_TRAKING/Documents/InvoicePieces.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\Desktop\Respaldo\Images\Datos Andres\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isaac\source\repos\AVT_TRAKING2\AVT_TRAKING-b5a19f52c2a889d8592336db032ecf143043f8f5\AVT_TRAKING\AVT_TRAKING\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12579EE-93E7-45BF-B2BF-BA4B59092DDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE776276-DA66-468F-BF09-16D2136E4355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7815" yWindow="1125" windowWidth="12555" windowHeight="5895" activeTab="1" xr2:uid="{38B5D577-474C-4399-9CA6-7E2D0DD88AA4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{38B5D577-474C-4399-9CA6-7E2D0DD88AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Pieces" sheetId="3" r:id="rId1"/>
     <sheet name="SRLs" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="Consulta_desde_VRT_TRAKING" localSheetId="0" hidden="1">Pieces!$A$5:$L$14</definedName>
+    <definedName name="Consulta_desde_VRT_TRAKING" localSheetId="0" hidden="1">Pieces!$A$5:$M$7</definedName>
     <definedName name="Consulta_desde_VRT_TRAKING" localSheetId="1" hidden="1">SRLs!$A$5:$H$7</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -42,10 +42,10 @@
   <connection id="1" xr16:uid="{CC493693-2191-4FE3-9290-BF7A0F801683}" keepAlive="1" name="Consulta - InvoiceExcel" description="Conexión a la consulta 'InvoiceExcel' en el libro." type="5" refreshedVersion="7" background="1" saveData="1">
     <dbPr connection="Provider=Microsoft.Mashup.OleDb.1;Data Source=$Workbook$;Location=InvoiceExcel;Extended Properties=&quot;&quot;" command="SELECT * FROM [InvoiceExcel]"/>
   </connection>
-  <connection id="2" xr16:uid="{358B69CF-9515-41AB-97DE-7160754EFFB3}" name="Consulta desde VRT_TRAKING" type="1" refreshedVersion="7" background="1" refreshOnLoad="1" saveData="1">
-    <dbPr connection="DRIVER=SQL Server;SERVER=127.0.0.1;UID=isaac;Trusted_Connection=Yes;APP=Microsoft Office;WSID=DESKTOP-S806JIQ;DATABASE=VRT_TRAKING" command="SELECT InvoiceExcel.&quot;Labor WO / NERWORK #&quot;, InvoiceExcel.&quot;Type (O,M,T,C)&quot;, InvoiceExcel.&quot;Tag #&quot;, InvoiceExcel.Pieces, InvoiceExcel.UNIT, InvoiceExcel.Location, InvoiceExcel.&quot;Date UP&quot;, InvoiceExcel.&quot;Date Down&quot;, InvoiceExcel.&quot;Invoice Amount&quot;, InvoiceExcel.ACTIVEDAYS, InvoiceExcel.RDays, InvoiceExcel.Work_x000d__x000a_FROM VRT_TRAKING.dbo.InvoiceExcel InvoiceExcel_x000d__x000a_ORDER BY InvoiceExcel.&quot;Tag #&quot;"/>
+  <connection id="2" xr16:uid="{358B69CF-9515-41AB-97DE-7160754EFFB3}" name="Consulta desde VRT_TRAKING" type="1" refreshedVersion="8" background="1" refreshOnLoad="1" saveData="1">
+    <dbPr connection="DRIVER=SQL Server;SERVER=127.0.0.1;UID=isaac;Trusted_Connection=Yes;APP=Microsoft Office;WSID=DESKTOP-S806JIQ;DATABASE=VRT_TRAKING" command="SELECT InvoiceExcel.&quot;Labor WO / Network #&quot;, InvoiceExcel.&quot;Type (O,M,T,C)&quot;, InvoiceExcel.&quot;Tag #&quot;, InvoiceExcel.Pieces, InvoiceExcel.UNIT, InvoiceExcel.Location, InvoiceExcel.&quot;Date UP&quot;, InvoiceExcel.&quot;Date Down&quot;, InvoiceExcel.&quot;Invoice Amount&quot;, InvoiceExcel.ACTIVEDAYS, InvoiceExcel.RDays, InvoiceExcel.Work_x000d__x000a_FROM VRT_TRAKING.dbo.InvoiceExcel InvoiceExcel_x000d__x000a_ORDER BY InvoiceExcel.&quot;Tag #&quot;"/>
   </connection>
-  <connection id="3" xr16:uid="{EE09C335-DAC7-4B93-B309-92AFA520840C}" name="Consulta desde VRT_TRAKING1" type="1" refreshedVersion="7" background="1" refreshOnLoad="1" saveData="1">
+  <connection id="3" xr16:uid="{EE09C335-DAC7-4B93-B309-92AFA520840C}" name="Consulta desde VRT_TRAKING1" type="1" refreshedVersion="8" background="1" refreshOnLoad="1" saveData="1">
     <dbPr connection="DRIVER=SQL Server;SERVER=127.0.0.1;UID=isaac;Trusted_Connection=Yes;APP=Microsoft Office;WSID=DESKTOP-S806JIQ;DATABASE=VRT_TRAKING" command="SELECT InvoiceExcelYOYOS.&quot;Labor WO / Network #&quot;, InvoiceExcelYOYOS.&quot;Type (O,M,T,C)&quot;, InvoiceExcelYOYOS.&quot;Tag #&quot;, InvoiceExcelYOYOS.Pieces, InvoiceExcelYOYOS.UNIT, InvoiceExcelYOYOS.Location, InvoiceExcelYOYOS.&quot;Date UP&quot;, InvoiceExcelYOYOS.&quot;Date Down&quot;_x000d__x000a_FROM VRT_TRAKING.dbo.InvoiceExcelYOYOS InvoiceExcelYOYOS_x000d__x000a_ORDER BY InvoiceExcelYOYOS.&quot;Tag #&quot;"/>
   </connection>
   <connection id="4" xr16:uid="{32D1275F-F463-4C03-B5B4-F70030FC115D}" odcFile="C:\Users\isaac\Documents\Mis archivos de origen de datos\localhost VRT_TRAKING product.odc" keepAlive="1" name="localhost VRT_TRAKING product" type="5" refreshedVersion="0" new="1" background="1">
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
   <si>
     <t>Type (O,M,T,C)</t>
   </si>
@@ -96,57 +96,15 @@
     <t>01/04/2022</t>
   </si>
   <si>
-    <t>1142</t>
-  </si>
-  <si>
-    <t>3348628</t>
-  </si>
-  <si>
-    <t>1143</t>
-  </si>
-  <si>
-    <t>P1FIN A Micronizing</t>
-  </si>
-  <si>
-    <t>3348700</t>
-  </si>
-  <si>
-    <t>1146</t>
-  </si>
-  <si>
-    <t>P2TICL Purification</t>
-  </si>
-  <si>
-    <t>01/07/2022</t>
-  </si>
-  <si>
-    <t>3348495</t>
-  </si>
-  <si>
-    <t>1145</t>
-  </si>
-  <si>
-    <t>P1TICL Refrigeration</t>
-  </si>
-  <si>
-    <t>01/06/2022</t>
-  </si>
-  <si>
     <t>Build</t>
   </si>
   <si>
     <t>1140</t>
   </si>
   <si>
-    <t>01/03/2021</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>Labor WO / NERWORK #</t>
-  </si>
-  <si>
     <t>Tag #</t>
   </si>
   <si>
@@ -178,6 +136,15 @@
   </si>
   <si>
     <t>01/03/2022</t>
+  </si>
+  <si>
+    <t>1139</t>
+  </si>
+  <si>
+    <t>03/01/2022</t>
+  </si>
+  <si>
+    <t>SRLs</t>
   </si>
 </sst>
 </file>
@@ -366,19 +333,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -407,6 +367,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -426,7 +388,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
         <strike val="0"/>
@@ -447,12 +409,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -489,13 +445,13 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Consulta desde VRT_TRAKING" refreshOnLoad="1" connectionId="2" xr16:uid="{57C86AB9-C581-4EF6-BD03-288C1BFB418E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="13">
-    <queryTableFields count="12">
-      <queryTableField id="1" name="Labor WO / NERWORK #" tableColumnId="1"/>
+  <queryTableRefresh nextId="15">
+    <queryTableFields count="13">
       <queryTableField id="2" name="Type (O,M,T,C)" tableColumnId="2"/>
       <queryTableField id="3" name="Tag #" tableColumnId="3"/>
       <queryTableField id="4" name="Pieces" tableColumnId="4"/>
       <queryTableField id="5" name="UNIT" tableColumnId="5"/>
+      <queryTableField id="14" dataBound="0" tableColumnId="13"/>
       <queryTableField id="6" name="Location" tableColumnId="6"/>
       <queryTableField id="7" name="Date UP" tableColumnId="7"/>
       <queryTableField id="8" name="Date Down" tableColumnId="8"/>
@@ -503,6 +459,7 @@
       <queryTableField id="10" name="ACTIVEDAYS" tableColumnId="10"/>
       <queryTableField id="11" name="RDays" tableColumnId="11"/>
       <queryTableField id="12" name="Work" tableColumnId="12"/>
+      <queryTableField id="13" name="Labor WO / Network #" tableColumnId="1"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -526,13 +483,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0D176718-B392-4A9D-9070-4B0EE3EA7DDC}" name="Tabla_Consulta_desde_VRT_TRAKING" displayName="Tabla_Consulta_desde_VRT_TRAKING" ref="A5:L15" tableType="queryTable" totalsRowCount="1" headerRowDxfId="3">
-  <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{A1400F7A-234C-4C8B-B435-3F88501FD8B7}" uniqueName="1" name="Labor WO / NERWORK #" queryTableFieldId="1" dataDxfId="2" totalsRowDxfId="1"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0D176718-B392-4A9D-9070-4B0EE3EA7DDC}" name="Tabla_Consulta_desde_VRT_TRAKING" displayName="Tabla_Consulta_desde_VRT_TRAKING" ref="A5:M8" tableType="queryTable" totalsRowCount="1" headerRowDxfId="1">
+  <tableColumns count="13">
     <tableColumn id="2" xr3:uid="{45B8D241-B5C8-4158-8A96-974711A7D544}" uniqueName="2" name="Type (O,M,T,C)" queryTableFieldId="2"/>
     <tableColumn id="3" xr3:uid="{C55F0CFC-4D16-42B3-9FF5-44F287BD50D2}" uniqueName="3" name="Tag #" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{53007AC2-912B-487D-BC00-D1306BC03F21}" uniqueName="4" name="Pieces" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{0638C9D9-DFED-43E8-8D02-F494A1A695F4}" uniqueName="5" name="UNIT" queryTableFieldId="5"/>
+    <tableColumn id="13" xr3:uid="{FD606018-A8B7-4EE8-9801-01CD60715289}" uniqueName="13" name="SRLs" queryTableFieldId="14"/>
     <tableColumn id="6" xr3:uid="{A1FC7E5C-2C57-41A0-B902-E363A52E75E0}" uniqueName="6" name="Location" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{D2A6E5EA-0830-401B-B814-878ECDF4E08E}" uniqueName="7" name="Date UP" queryTableFieldId="7"/>
     <tableColumn id="8" xr3:uid="{E3E4C361-4559-4927-A2B3-0943A518FCAA}" uniqueName="8" name="Date Down" queryTableFieldId="8"/>
@@ -540,6 +497,7 @@
     <tableColumn id="10" xr3:uid="{DE68B60D-1AE4-4C11-A2A6-E732056235A1}" uniqueName="10" name="ACTIVEDAYS" queryTableFieldId="10"/>
     <tableColumn id="11" xr3:uid="{0317DF1D-BAA4-408F-9374-DC661A60C2A9}" uniqueName="11" name="RDays" queryTableFieldId="11"/>
     <tableColumn id="12" xr3:uid="{B3D51080-ABCC-4A29-9907-A25ECC1D4EA8}" uniqueName="12" name="Work" queryTableFieldId="12"/>
+    <tableColumn id="1" xr3:uid="{C7BF29D3-C07F-4234-831A-200DE77CF914}" uniqueName="1" name="Labor WO / Network #" queryTableFieldId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -858,110 +816,120 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15DBB563-4785-449F-AAF5-1BCA63F1C3B4}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="21">
-        <v>44593</v>
-      </c>
-      <c r="K1" s="10"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="24">
-        <v>44620</v>
-      </c>
-      <c r="K2" s="25">
-        <f>J2-(J1-1)</f>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="18"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="10"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="29"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="18">
+        <v>44569</v>
+      </c>
+      <c r="L1" s="7"/>
+      <c r="M1" s="23"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="J2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="21">
+        <v>44569</v>
+      </c>
+      <c r="L2" s="22">
+        <f>K2-(K1-1)</f>
+        <v>1</v>
+      </c>
+      <c r="M2" s="24"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="19"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+      <c r="N3" s="14"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="20"/>
+      <c r="Q3" s="7"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="28"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>2</v>
@@ -970,13 +938,13 @@
         <v>3</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>5</v>
@@ -984,417 +952,151 @@
       <c r="L5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>7</v>
+      <c r="M5" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6">
-        <v>15</v>
-      </c>
-      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
         <v>28</v>
       </c>
       <c r="I6">
-        <v>3</v>
+        <v>0.09</v>
       </c>
       <c r="J6">
-        <v>462</v>
+        <v>57</v>
       </c>
       <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6" t="s">
         <v>10</v>
       </c>
-      <c r="L6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="M6" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
       <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="I7">
-        <v>0.3</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="J7">
-        <v>96</v>
+        <v>233</v>
       </c>
       <c r="K7">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M7" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8">
-        <v>0.8</v>
-      </c>
-      <c r="J8">
-        <v>96</v>
-      </c>
-      <c r="K8">
-        <v>10</v>
-      </c>
-      <c r="L8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9">
-        <v>0.6</v>
-      </c>
-      <c r="J9">
-        <v>96</v>
-      </c>
-      <c r="K9">
-        <v>10</v>
-      </c>
-      <c r="L9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10">
-        <v>3</v>
-      </c>
-      <c r="E10" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" t="s">
-        <v>28</v>
-      </c>
-      <c r="I10">
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="J10">
-        <v>96</v>
-      </c>
-      <c r="K10">
-        <v>10</v>
-      </c>
-      <c r="L10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11">
-        <v>1.2</v>
-      </c>
-      <c r="J11">
-        <v>96</v>
-      </c>
-      <c r="K11">
-        <v>10</v>
-      </c>
-      <c r="L11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12">
-        <v>35</v>
-      </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I12">
-        <v>6.4</v>
-      </c>
-      <c r="J12">
-        <v>94</v>
-      </c>
-      <c r="K12">
-        <v>10</v>
-      </c>
-      <c r="L12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" t="s">
-        <v>28</v>
-      </c>
-      <c r="I13">
-        <v>0.4</v>
-      </c>
-      <c r="J13">
-        <v>93</v>
-      </c>
-      <c r="K13">
-        <v>10</v>
-      </c>
-      <c r="L13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14" t="s">
-        <v>19</v>
-      </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" t="s">
-        <v>28</v>
-      </c>
-      <c r="I14">
-        <v>0.6</v>
-      </c>
-      <c r="J14">
-        <v>93</v>
-      </c>
-      <c r="K14">
-        <v>10</v>
-      </c>
-      <c r="L14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
+      <c r="A17" s="4"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
+      <c r="A18" s="4"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="4"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="4"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+      <c r="A21" s="4"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="6"/>
+      <c r="A22" s="4"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="4"/>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
+      <c r="A24" s="4"/>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="6"/>
+      <c r="A25" s="4"/>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
+      <c r="A26" s="4"/>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="6"/>
+      <c r="A27" s="4"/>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="6"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="6"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
+      <c r="A28" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="K4:O4"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="L4:Q4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1408,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F57257B-8A29-41E9-A359-4D17BE936CD4}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,88 +1127,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J1" s="13">
-        <v>44593</v>
+      <c r="A1" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="10">
+        <v>44569</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" s="16">
-        <v>44620</v>
-      </c>
-      <c r="K2" s="5"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="13">
+        <v>44569</v>
+      </c>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
-      <c r="J3" s="18"/>
+      <c r="A3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
+      <c r="A4" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="19" t="s">
+      <c r="C5" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="19" t="s">
+      <c r="E5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="20"/>
+      <c r="H5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1516,7 +1218,7 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -1528,10 +1230,10 @@
         <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="H6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -1557,7 +1259,7 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>